<commit_message>
Edicion de la carpeta requisitos
se agrego documento de lista de requisitos
</commit_message>
<xml_diff>
--- a/PROYECTOS/Proy_SSEL/Documentacion/3. Requisitos/SSEL-LR.xlsx
+++ b/PROYECTOS/Proy_SSEL/Documentacion/3. Requisitos/SSEL-LR.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulpin\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>N°</t>
   </si>
@@ -40,12 +45,6 @@
     <t>Registro de subastador</t>
   </si>
   <si>
-    <t>El sistema deberá almacenar la información de los participantes en la subasta</t>
-  </si>
-  <si>
-    <t>Debido a que se requiere tener un registro de los participantes en la subasta.</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
@@ -55,18 +54,12 @@
     <t>Registro de producto</t>
   </si>
   <si>
-    <t>El sistema deberá permitir registrar los productos a subastar</t>
-  </si>
-  <si>
     <t>Debido a que hay un producto por subastrar, se debe registrar las caracteristicas del producto</t>
   </si>
   <si>
     <t>Visualizar Subasta</t>
   </si>
   <si>
-    <t>El sistema deberá mostrar los producto que se estab subastanado</t>
-  </si>
-  <si>
     <t>Debido a que hay varios productos en subasta, se debe mostrar todos los productos que esta vigentes en la subasta</t>
   </si>
   <si>
@@ -100,9 +93,6 @@
     <t>Registrar Usuarios</t>
   </si>
   <si>
-    <t>El sistema deberá almacenar el registro de los usuarios que deseen participar en la subasta</t>
-  </si>
-  <si>
     <t>Debido a que cualquier usuario puede participar en cualquier subasta</t>
   </si>
   <si>
@@ -218,6 +208,39 @@
   </si>
   <si>
     <t>RNF-14</t>
+  </si>
+  <si>
+    <t>CASO DE USO</t>
+  </si>
+  <si>
+    <t>Apostar</t>
+  </si>
+  <si>
+    <t>Registrar en sistema</t>
+  </si>
+  <si>
+    <t>Subastar Producto</t>
+  </si>
+  <si>
+    <t>Autenticar</t>
+  </si>
+  <si>
+    <t>Visualizar subasta</t>
+  </si>
+  <si>
+    <t>El sistema deberá registrar el nombre, codigo subastador, item producto, categoria.</t>
+  </si>
+  <si>
+    <t>Debido a que se requiere tener un registro de los participantes que subastan su producto.</t>
+  </si>
+  <si>
+    <t>El sistema deberá registra el rnombre, dni, numero de cuenta, correo, direccion, ID de los usuarios que deseen participar en la subasta</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitir registrar datos del productos (nombre, categoria, fecha inicio subasta, fecha de caducidad, precio base) a subastar</t>
+  </si>
+  <si>
+    <t>El sistema deberá mostrar los producto que se esta subastanado</t>
   </si>
 </sst>
 </file>
@@ -225,7 +248,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_ &quot;€&quot;* #,##0.00_ ;_ &quot;€&quot;* \-#,##0.00_ ;_ &quot;€&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;* #,##0.00_ ;_ &quot;€&quot;* \-#,##0.00_ ;_ &quot;€&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -272,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -304,12 +327,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -346,10 +395,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,7 +732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -682,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G24"/>
+  <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -699,10 +757,10 @@
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -711,7 +769,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
@@ -733,8 +791,11 @@
       <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -742,359 +803,380 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H5" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>55</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edicion Lista de Requitos
Mejorando lista de requisitos
</commit_message>
<xml_diff>
--- a/PROYECTOS/Proy_SSEL/Documentacion/3. Requisitos/SSEL-LR.xlsx
+++ b/PROYECTOS/Proy_SSEL/Documentacion/3. Requisitos/SSEL-LR.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulpin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulpin\Documents\GitHub\FISIDEVELOPS-G3\PROYECTOS\Proy_SSEL\Documentacion\3. Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lista de Requisitos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -398,11 +398,11 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -759,15 +759,15 @@
   <sheetData>
     <row r="2" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
@@ -1019,7 +1019,7 @@
       <c r="G13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1043,7 +1043,7 @@
       <c r="G14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1067,7 +1067,7 @@
       <c r="G15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1091,7 +1091,7 @@
       <c r="G16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1115,7 +1115,7 @@
       <c r="G17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1139,7 +1139,7 @@
       <c r="G18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>

</xml_diff>